<commit_message>
fixed site laglong errors
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2015/NW Appledore 2015/NWAppledore_siteinfo_2015.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2015/NW Appledore 2015/NWAppledore_siteinfo_2015.xlsx
@@ -146,8 +146,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -186,7 +192,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -197,6 +203,9 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -207,6 +216,9 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -539,7 +551,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -743,10 +755,10 @@
         <v>42.991222590207997</v>
       </c>
       <c r="J4">
+        <v>-70.618192534893694</v>
+      </c>
+      <c r="K4">
         <v>42.991071380674803</v>
-      </c>
-      <c r="K4">
-        <v>-70.618192534893694</v>
       </c>
       <c r="L4">
         <v>-70.618612384423599</v>

</xml_diff>